<commit_message>
Updated version number. Minor modification to examples.
</commit_message>
<xml_diff>
--- a/examples/VASP_to_thermdat/example1/thermdat_input.xlsx
+++ b/examples/VASP_to_thermdat/example1/thermdat_input.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\UDel Documents\UDel Research\Github\PyMuTT\examples\VASP_to_thermdat\example1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\UDel Documents\UDel Research\Github\pMuTT\examples\VASP_to_thermdat\example1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8A2C001-4A93-4573-8A83-8AC4068D63EC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2AE9804-80C9-479F-8082-8C7824A505E0}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5352" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="39">
   <si>
     <t>name</t>
   </si>
@@ -114,9 +114,6 @@
     <t>Harmonic</t>
   </si>
   <si>
-    <t>Type of thermodynamic model. Supported options include IdealGas and Harmonic</t>
-  </si>
-  <si>
     <t>.\H2O\CONTCAR</t>
   </si>
   <si>
@@ -139,6 +136,12 @@
   </si>
   <si>
     <t>statmech_model</t>
+  </si>
+  <si>
+    <t>Electronic</t>
+  </si>
+  <si>
+    <t>Type of thermodynamic model. See presets available here: https://vlachosgroup.github.io/pMuTT/statmech.html?highlight=presets#presets</t>
   </si>
 </sst>
 </file>
@@ -529,16 +532,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>37</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>2</v>
@@ -553,13 +556,13 @@
         <v>5</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
@@ -583,7 +586,7 @@
         <v>25</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>11</v>
@@ -634,7 +637,7 @@
         <v>-14.2209</v>
       </c>
       <c r="H3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I3">
         <v>2</v>
@@ -675,7 +678,7 @@
         <v>-6.7598000000000003</v>
       </c>
       <c r="H4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I4">
         <v>2</v>
@@ -710,7 +713,7 @@
         <v>-9.86</v>
       </c>
       <c r="H5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I5">
         <v>2</v>
@@ -805,7 +808,7 @@
         <v>1</v>
       </c>
       <c r="F8" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="G8">
         <v>7</v>
@@ -892,7 +895,7 @@
         <v>1</v>
       </c>
       <c r="F11" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="G11">
         <v>7</v>

</xml_diff>